<commit_message>
Atualiza os processos da pasta DATA
</commit_message>
<xml_diff>
--- a/data/compras-coronavirus.xlsx
+++ b/data/compras-coronavirus.xlsx
@@ -1143,6 +1143,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C7" s="2">
         <v>43936</v>
       </c>
@@ -1267,6 +1272,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C8" s="2">
         <v>43936</v>
       </c>
@@ -1391,6 +1401,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C9" s="2">
         <v>43936</v>
       </c>
@@ -1515,6 +1530,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C10" s="2">
         <v>43936</v>
       </c>
@@ -1639,6 +1659,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C11" s="2">
         <v>43936</v>
       </c>
@@ -1763,6 +1788,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C12" s="2">
         <v>43936</v>
       </c>
@@ -1887,6 +1917,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C13" s="2">
         <v>43936</v>
       </c>
@@ -2011,6 +2046,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C14" s="2">
         <v>43936</v>
       </c>
@@ -2135,6 +2175,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C15" s="2">
         <v>43936</v>
       </c>
@@ -2259,6 +2304,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C16" s="2">
         <v>43936</v>
       </c>
@@ -2383,6 +2433,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C17" s="2">
         <v>43936</v>
       </c>
@@ -2507,6 +2562,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C18" s="2">
         <v>43936</v>
       </c>
@@ -2631,6 +2691,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C19" s="2">
         <v>43936</v>
       </c>
@@ -2755,6 +2820,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C20" s="2">
         <v>43936</v>
       </c>
@@ -2879,6 +2949,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C21" s="2">
         <v>43936</v>
       </c>
@@ -3003,6 +3078,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C22" s="2">
         <v>43936</v>
       </c>
@@ -3127,6 +3207,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C23" s="2">
         <v>43936</v>
       </c>
@@ -3251,6 +3336,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C24" s="2">
         <v>43936</v>
       </c>
@@ -3375,6 +3465,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C25" s="2">
         <v>43936</v>
       </c>
@@ -3499,6 +3594,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C26" s="2">
         <v>43936</v>
       </c>
@@ -3623,6 +3723,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C27" s="2">
         <v>43936</v>
       </c>
@@ -3747,6 +3852,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C28" s="2">
         <v>43936</v>
       </c>
@@ -3871,6 +3981,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C29" s="2">
         <v>43936</v>
       </c>
@@ -3995,6 +4110,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C30" s="2">
         <v>43936</v>
       </c>
@@ -4119,6 +4239,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C31" s="2">
         <v>43936</v>
       </c>
@@ -4243,6 +4368,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C32" s="2">
         <v>43936</v>
       </c>
@@ -4367,6 +4497,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C33" s="2">
         <v>43936</v>
       </c>
@@ -4491,6 +4626,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C34" s="2">
         <v>43936</v>
       </c>
@@ -4615,6 +4755,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C35" s="2">
         <v>43936</v>
       </c>
@@ -4739,6 +4884,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C36" s="2">
         <v>43936</v>
       </c>
@@ -4863,6 +5013,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C37" s="2">
         <v>43936</v>
       </c>
@@ -4987,6 +5142,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C38" s="2">
         <v>43936</v>
       </c>
@@ -5111,6 +5271,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C39" s="2">
         <v>43936</v>
       </c>
@@ -5235,6 +5400,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C40" s="2">
         <v>43936</v>
       </c>
@@ -5359,6 +5529,11 @@
           <t>0250073 000004/2020</t>
         </is>
       </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/17466/0/0/0/0/16388/59750367/107136/1252305/322690/0250073000004-2020</t>
+        </is>
+      </c>
       <c r="C41" s="2">
         <v>43936</v>
       </c>
@@ -5590,6 +5765,11 @@
           <t>0250073 000009/2020</t>
         </is>
       </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831094/0/0/8783/0/0/0/0/5444/66403693/29886/415812/322918/0250073000009-2020</t>
+        </is>
+      </c>
       <c r="C43" s="2">
         <v>43942</v>
       </c>
@@ -8168,6 +8348,11 @@
           <t>1250084 000010/2020</t>
         </is>
       </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831094/0/0/61994/0/0/0/0/21797/84950030/216609/1754467/322336/1250084000010-2020</t>
+        </is>
+      </c>
       <c r="C67" s="2">
         <v>43930</v>
       </c>
@@ -12305,6 +12490,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C104" s="2">
         <v>43910</v>
       </c>
@@ -12429,6 +12619,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C105" s="2">
         <v>43910</v>
       </c>
@@ -12553,6 +12748,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C106" s="2">
         <v>43910</v>
       </c>
@@ -12677,6 +12877,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C107" s="2">
         <v>43910</v>
       </c>
@@ -12801,6 +13006,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C108" s="2">
         <v>43910</v>
       </c>
@@ -12925,6 +13135,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C109" s="2">
         <v>43910</v>
       </c>
@@ -13049,6 +13264,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C110" s="2">
         <v>43910</v>
       </c>
@@ -13173,6 +13393,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C111" s="2">
         <v>43910</v>
       </c>
@@ -13297,6 +13522,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C112" s="2">
         <v>43910</v>
       </c>
@@ -13421,6 +13651,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C113" s="2">
         <v>43910</v>
       </c>
@@ -13545,6 +13780,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C114" s="2">
         <v>43910</v>
       </c>
@@ -13669,6 +13909,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C115" s="2">
         <v>43910</v>
       </c>
@@ -13793,6 +14038,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C116" s="2">
         <v>43910</v>
       </c>
@@ -13917,6 +14167,11 @@
           <t>1501561 000005/2020</t>
         </is>
       </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/0/0/0/17532/0/0/0/0/21609/84950013/170590/1672541</t>
+        </is>
+      </c>
       <c r="C117" s="2">
         <v>43910</v>
       </c>
@@ -14041,6 +14296,11 @@
           <t>1501561 000006/2020</t>
         </is>
       </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-filtros/5/2020/01-01-2020/30-04-2020/65/65888</t>
+        </is>
+      </c>
       <c r="C118" s="2">
         <v>43912</v>
       </c>
@@ -14165,6 +14425,11 @@
           <t>1501561 000009/2020</t>
         </is>
       </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-filtros/5/2020/01-01-2020/30-04-2020/65/65898</t>
+        </is>
+      </c>
       <c r="C119" s="2">
         <v>43916</v>
       </c>
@@ -14289,6 +14554,11 @@
           <t>1501561 000010/2020</t>
         </is>
       </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-filtros/5/2020/01-01-2020/30-04-2020/65/65894</t>
+        </is>
+      </c>
       <c r="C120" s="2">
         <v>43916</v>
       </c>
@@ -14948,6 +15218,11 @@
           <t>1501561 000015/2020</t>
         </is>
       </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-filtros/5/2020/01-01-2020/31-05-2020/12/65960</t>
+        </is>
+      </c>
       <c r="C126" s="2">
         <v>43923</v>
       </c>
@@ -15072,6 +15347,11 @@
           <t>1501561 000016/2020</t>
         </is>
       </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831017/0/0/17532/0/0/0/0/10733/65320034/10036/125628/321781/1501561000016-2020</t>
+        </is>
+      </c>
       <c r="C127" s="2">
         <v>43924</v>
       </c>
@@ -15196,6 +15476,11 @@
           <t>1501561 000017/2020</t>
         </is>
       </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-filtros/5/2020/01-01-2020/31-05-2020/12/65986</t>
+        </is>
+      </c>
       <c r="C128" s="2">
         <v>43924</v>
       </c>
@@ -15534,6 +15819,11 @@
           <t>1501561 000019/2020</t>
         </is>
       </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831017/0/0/9190/0/0/0/0/1547/65181220/167591/1649256/322108/1501561000019-2020</t>
+        </is>
+      </c>
       <c r="C131" s="2">
         <v>43929</v>
       </c>
@@ -15658,6 +15948,11 @@
           <t>1501561 000020/2020</t>
         </is>
       </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831065/0/0/17532/0/0/0/0/10733/65320034/10036/125628/322112/1501561000020-2020</t>
+        </is>
+      </c>
       <c r="C132" s="2">
         <v>43930</v>
       </c>
@@ -15782,6 +16077,11 @@
           <t>1501561 000020/2020</t>
         </is>
       </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831065/0/0/17532/0/0/0/0/10733/65320034/10036/125628/322112/1501561000020-2020</t>
+        </is>
+      </c>
       <c r="C133" s="2">
         <v>43930</v>
       </c>
@@ -15906,6 +16206,11 @@
           <t>1501561 000020/2020</t>
         </is>
       </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831065/0/0/17532/0/0/0/0/10733/65320034/10036/125628/322112/1501561000020-2020</t>
+        </is>
+      </c>
       <c r="C134" s="2">
         <v>43930</v>
       </c>
@@ -16030,6 +16335,11 @@
           <t>1501561 000020/2020</t>
         </is>
       </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831065/0/0/17532/0/0/0/0/10733/65320034/10036/125628/322112/1501561000020-2020</t>
+        </is>
+      </c>
       <c r="C135" s="2">
         <v>43930</v>
       </c>
@@ -16154,6 +16464,11 @@
           <t>1501561 000020/2020</t>
         </is>
       </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831065/0/0/17532/0/0/0/0/10733/65320034/10036/125628/322112/1501561000020-2020</t>
+        </is>
+      </c>
       <c r="C136" s="2">
         <v>43930</v>
       </c>
@@ -16278,6 +16593,11 @@
           <t>1501561 000020/2020</t>
         </is>
       </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831065/0/0/17532/0/0/0/0/10733/65320034/10036/125628/322112/1501561000020-2020</t>
+        </is>
+      </c>
       <c r="C137" s="2">
         <v>43930</v>
       </c>
@@ -16402,6 +16722,11 @@
           <t>1501561 000020/2020</t>
         </is>
       </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831065/0/0/17532/0/0/0/0/10733/65320034/10036/125628/322112/1501561000020-2020</t>
+        </is>
+      </c>
       <c r="C138" s="2">
         <v>43930</v>
       </c>
@@ -16526,6 +16851,11 @@
           <t>1501561 000021/2020</t>
         </is>
       </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-filtros/5/2020/01-01-2020/31-05-2020/12/66043</t>
+        </is>
+      </c>
       <c r="C139" s="2">
         <v>43930</v>
       </c>
@@ -16650,6 +16980,11 @@
           <t>1501561 000022/2020</t>
         </is>
       </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831017/0/0/9190/0/0/0/0/1547/65181220/167591/1649256/322108/1501561000019-2020</t>
+        </is>
+      </c>
       <c r="C140" s="2">
         <v>43934</v>
       </c>
@@ -17202,6 +17537,11 @@
           <t>1501561 000025/2020</t>
         </is>
       </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831065/0/0/17532/0/0/0/0/10733/65320034/10036/125628/322631/1501561000025-2020</t>
+        </is>
+      </c>
       <c r="C145" s="2">
         <v>43938</v>
       </c>
@@ -17326,6 +17666,11 @@
           <t>1501561 000026/2020</t>
         </is>
       </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831065/0/0/30348/0/0/0/0/10733/65320034/8733/125245/322692/1501561000026-2020</t>
+        </is>
+      </c>
       <c r="C146" s="2">
         <v>43938</v>
       </c>
@@ -17450,6 +17795,11 @@
           <t>1501561 000026/2020</t>
         </is>
       </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831065/0/0/30348/0/0/0/0/10733/65320034/8733/125245/322692/1501561000026-2020</t>
+        </is>
+      </c>
       <c r="C147" s="2">
         <v>43938</v>
       </c>
@@ -17681,6 +18031,11 @@
           <t>1501561 000028/2020</t>
         </is>
       </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-04-2020/30-06-2020/1831017/0/0/239/0/0/0/0/822/65181751/215727/1753681/323054/1501561000028-2020</t>
+        </is>
+      </c>
       <c r="C149" s="2">
         <v>43948</v>
       </c>
@@ -17805,6 +18160,11 @@
           <t>1501561 000028/2020</t>
         </is>
       </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-04-2020/30-06-2020/1831017/0/0/239/0/0/0/0/822/65181751/215727/1753681/323054/1501561000028-2020</t>
+        </is>
+      </c>
       <c r="C150" s="2">
         <v>43948</v>
       </c>
@@ -17929,6 +18289,11 @@
           <t>1501561 000029/2020</t>
         </is>
       </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-04-2020/30-06-2020/1831017/0/0/20981/0/0/0/0/3854/68201451/215959/1753924/323117/1501561000029-2020</t>
+        </is>
+      </c>
       <c r="C151" s="2">
         <v>43950</v>
       </c>
@@ -18053,6 +18418,11 @@
           <t>1501561 000029/2020</t>
         </is>
       </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-04-2020/30-06-2020/1831017/0/0/20981/0/0/0/0/3854/68201451/215959/1753924/323117/1501561000029-2020</t>
+        </is>
+      </c>
       <c r="C152" s="2">
         <v>43950</v>
       </c>
@@ -18177,6 +18547,11 @@
           <t>1501561 000029/2020</t>
         </is>
       </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-04-2020/30-06-2020/1831017/0/0/20981/0/0/0/0/3854/68201451/215959/1753924/323117/1501561000029-2020</t>
+        </is>
+      </c>
       <c r="C153" s="2">
         <v>43950</v>
       </c>
@@ -18301,6 +18676,11 @@
           <t>1501561 000029/2020</t>
         </is>
       </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-04-2020/30-06-2020/1831017/0/0/20981/0/0/0/0/3854/68201451/215959/1753924/323117/1501561000029-2020</t>
+        </is>
+      </c>
       <c r="C154" s="2">
         <v>43950</v>
       </c>
@@ -18425,6 +18805,11 @@
           <t>1501561 000029/2020</t>
         </is>
       </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-04-2020/30-06-2020/1831017/0/0/20981/0/0/0/0/3854/68201451/215959/1753924/323117/1501561000029-2020</t>
+        </is>
+      </c>
       <c r="C155" s="2">
         <v>43950</v>
       </c>
@@ -18549,6 +18934,11 @@
           <t>1501561 000030/2020</t>
         </is>
       </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-04-2020/30-06-2020/1831065/0/0/62110/0/0/0/0/15771/65320018/217626/1755366/323445/1501561000030-2020</t>
+        </is>
+      </c>
       <c r="C156" s="2">
         <v>43955</v>
       </c>
@@ -18673,6 +19063,11 @@
           <t>1501561 000031/2020</t>
         </is>
       </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-04-2020/30-06-2020/1831017/0/0/37380/0/0/0/0/822/65181751/219609/1758063/323435/1501561000031-2020</t>
+        </is>
+      </c>
       <c r="C157" s="2">
         <v>43956</v>
       </c>
@@ -18797,6 +19192,11 @@
           <t>1501561 000032/2020</t>
         </is>
       </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-04-2020/30-06-2020/1831008/0/0/62110/0/0/0/0/15771/65320018/217626/1755366/323606/1501561000032-2020</t>
+        </is>
+      </c>
       <c r="C158" s="2">
         <v>43959</v>
       </c>
@@ -19028,6 +19428,11 @@
           <t>2012015 000034/2020</t>
         </is>
       </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/covid-19/compras-contratos/contratoscovid-detalharcompra/322908</t>
+        </is>
+      </c>
       <c r="C160" s="2">
         <v>43921</v>
       </c>
@@ -22283,6 +22688,11 @@
           <t>2301925 000001/2020</t>
         </is>
       </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831084/0/0/19962/0/0/0/0/7051/3010163/94368/1155/321506/2301925000001-2020</t>
+        </is>
+      </c>
       <c r="C188" s="2">
         <v>43921</v>
       </c>
@@ -22410,6 +22820,11 @@
           <t>2301925 000002/2020</t>
         </is>
       </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831084/0/0/16018/0/0/0/0/7051/3010163/94368/1155/322267/2301925000002-2020</t>
+        </is>
+      </c>
       <c r="C189" s="2">
         <v>43935</v>
       </c>
@@ -22532,6 +22947,11 @@
           <t>2301925 000003/2020</t>
         </is>
       </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/31-05-2020/1831084/0/0/26247/0/0/0/0/7051/3010163/94368/1155/323729/2301925000003-2020</t>
+        </is>
+      </c>
       <c r="C190" s="2">
         <v>43963</v>
       </c>
@@ -22659,6 +23079,11 @@
           <t>2311076 000134/2020</t>
         </is>
       </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831059/0/0/13609/0/0/0/0/8131/41300068/5218/18228/322585/2311076000134-2020</t>
+        </is>
+      </c>
       <c r="C191" s="2">
         <v>43928</v>
       </c>
@@ -22786,6 +23211,11 @@
           <t>2311076 000134/2020</t>
         </is>
       </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831059/0/0/13609/0/0/0/0/8131/41300068/5218/18228/322585/2311076000134-2020</t>
+        </is>
+      </c>
       <c r="C192" s="2">
         <v>43928</v>
       </c>
@@ -22913,6 +23343,11 @@
           <t>2311076 000134/2020</t>
         </is>
       </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831059/0/0/13609/0/0/0/0/8131/41300068/5218/18228/322585/2311076000134-2020</t>
+        </is>
+      </c>
       <c r="C193" s="2">
         <v>43928</v>
       </c>
@@ -23040,6 +23475,11 @@
           <t>2311076 000134/2020</t>
         </is>
       </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831059/0/0/13609/0/0/0/0/8131/41300068/5218/18228/322585/2311076000134-2020</t>
+        </is>
+      </c>
       <c r="C194" s="2">
         <v>43928</v>
       </c>
@@ -23167,6 +23607,11 @@
           <t>2311076 000134/2020</t>
         </is>
       </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831059/0/0/13609/0/0/0/0/8131/41300068/5218/18228/322585/2311076000134-2020</t>
+        </is>
+      </c>
       <c r="C195" s="2">
         <v>43928</v>
       </c>
@@ -23294,6 +23739,11 @@
           <t>2311076 000134/2020</t>
         </is>
       </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831059/0/0/13609/0/0/0/0/8131/41300068/5218/18228/322585/2311076000134-2020</t>
+        </is>
+      </c>
       <c r="C196" s="2">
         <v>43928</v>
       </c>
@@ -23419,6 +23869,11 @@
       <c r="A197" t="inlineStr">
         <is>
           <t>2311076 000134/2020</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/compras-e-patrimonio/compras-e-contratos/comprasecontratos-procedimento/3/2020/01-01-2020/30-04-2020/1831059/0/0/13609/0/0/0/0/8131/41300068/5218/18228/322585/2311076000134-2020</t>
         </is>
       </c>
       <c r="C197" s="2">

</xml_diff>

<commit_message>
Inclui processo de dispensa da Hemominas
</commit_message>
<xml_diff>
--- a/data/compras-coronavirus.xlsx
+++ b/data/compras-coronavirus.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF213"/>
+  <dimension ref="A1:AF214"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4098,10 +4098,10 @@
         <v>1.89</v>
       </c>
       <c r="AE29">
-        <v>75.60000000000001</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="AF29">
-        <v>75.60000000000001</v>
+        <v>75.59999999999999</v>
       </c>
     </row>
     <row r="30">
@@ -5874,7 +5874,7 @@
         <v>264850</v>
       </c>
       <c r="AC43">
-        <v>0.5700000000000001</v>
+        <v>0.57</v>
       </c>
       <c r="AD43">
         <v>0.38</v>
@@ -6730,16 +6730,16 @@
         <v>1</v>
       </c>
       <c r="AC51">
-        <v>8929.800000000001</v>
+        <v>8929.799999999999</v>
       </c>
       <c r="AD51">
-        <v>8929.800000000001</v>
+        <v>8929.799999999999</v>
       </c>
       <c r="AE51">
-        <v>8929.800000000001</v>
+        <v>8929.799999999999</v>
       </c>
       <c r="AF51">
-        <v>8929.800000000001</v>
+        <v>8929.799999999999</v>
       </c>
     </row>
     <row r="52">
@@ -6950,10 +6950,10 @@
         <v>1631.8</v>
       </c>
       <c r="AE53">
-        <v>4895.400000000001</v>
+        <v>4895.4</v>
       </c>
       <c r="AF53">
-        <v>4895.400000000001</v>
+        <v>4895.4</v>
       </c>
     </row>
     <row r="54">
@@ -11593,7 +11593,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D__x000D_
+          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D_
 contra Pânico e Incêndio e material para orientações de segurança.</t>
         </is>
       </c>
@@ -11723,7 +11723,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D__x000D_
+          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D_
 contra Pânico e Incêndio e material para orientações de segurança.</t>
         </is>
       </c>
@@ -11853,7 +11853,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D__x000D_
+          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D_
 contra Pânico e Incêndio e material para orientações de segurança.</t>
         </is>
       </c>
@@ -11983,7 +11983,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D__x000D_
+          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D_
 contra Pânico e Incêndio e material para orientações de segurança.</t>
         </is>
       </c>
@@ -12113,7 +12113,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D__x000D_
+          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D_
 contra Pânico e Incêndio e material para orientações de segurança.</t>
         </is>
       </c>
@@ -12243,7 +12243,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D__x000D_
+          <t>Compra emergencial de materiais para enfrentamento ao COVID-19. Materiais de Prevenção e Segurança_x000D_
 contra Pânico e Incêndio e material para orientações de segurança.</t>
         </is>
       </c>
@@ -24040,7 +24040,32 @@
         </is>
       </c>
       <c r="J198">
-        <v>0</v>
+        <v>9251383</v>
+      </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>https://www1.compras.mg.gov.br/contrato/gestaocontratos/arquivosContrato.html?idContrato=163606</t>
+        </is>
+      </c>
+      <c r="L198">
+        <v>2310</v>
+      </c>
+      <c r="M198" t="inlineStr">
+        <is>
+          <t>UNIVERSIDADE ESTADUAL DE MONTES CLAROS</t>
+        </is>
+      </c>
+      <c r="N198" s="2">
+        <v>44014</v>
+      </c>
+      <c r="O198" s="2">
+        <v>44013</v>
+      </c>
+      <c r="P198" s="2">
+        <v>44557</v>
+      </c>
+      <c r="Q198" s="2">
+        <v>44192</v>
       </c>
       <c r="R198" t="inlineStr">
         <is>
@@ -24120,7 +24145,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -24228,7 +24253,7 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -24336,7 +24361,7 @@
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -24444,7 +24469,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -24552,7 +24577,7 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -24660,7 +24685,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -24768,7 +24793,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -24876,7 +24901,7 @@
       </c>
       <c r="D206" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -24984,7 +25009,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -25092,7 +25117,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -25200,7 +25225,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -25308,7 +25333,7 @@
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -25416,7 +25441,7 @@
       </c>
       <c r="D211" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -25524,7 +25549,7 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -25632,7 +25657,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>Material de limpeza _x000D__x000D_
+          <t>Material de limpeza _x000D_
 SEI 2320.01.0004287/2020-78</t>
         </is>
       </c>
@@ -25722,6 +25747,113 @@
       </c>
       <c r="AF213">
         <v>6840</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2320310 000201/2020</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>http://www.transparencia.mg.gov.br/covid-19/compras-contratos/contratoscovid-detalharcompra/326183</t>
+        </is>
+      </c>
+      <c r="C214" s="2">
+        <v>44007</v>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>aquisição de painéis de proteção de acrílico para instalação nas Recepções e Cadastros das unidades</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>https://www1.compras.mg.gov.br/processocompra/processo/consultaProcessoCompra.html?metodo=pesquisar&amp;codigoUnidadeCompra=2320310&amp;numero=201&amp;ano=2020</t>
+        </is>
+      </c>
+      <c r="F214">
+        <v>2320</v>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>FUNDACAO CENTRO DE HEMATOLOGIA E HEMOTERAPIA DE MG</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>Dispensa de Licitação</t>
+        </is>
+      </c>
+      <c r="J214">
+        <v>0</v>
+      </c>
+      <c r="R214" t="inlineStr">
+        <is>
+          <t>19.173.186/0001-09</t>
+        </is>
+      </c>
+      <c r="S214" t="inlineStr">
+        <is>
+          <t>ACRILDAM INDUSTRIA E COMERCIO ARTEFATOS DE ACRILICO LTDA -EPP</t>
+        </is>
+      </c>
+      <c r="T214" t="inlineStr">
+        <is>
+          <t>2320.01.0007282/2020-14</t>
+        </is>
+      </c>
+      <c r="U214" t="inlineStr">
+        <is>
+          <t>https://www.sei.mg.gov.br/sei/modulos/pesquisa/md_pesq_processo_exibir.php?IC2o8Z7ACQH4LdQ4jJLJzjPBiLtP6l2FsQacllhUf-duzEubalut9yvd8-CzYYNLu7pd-wiM0k633-D6khhQNfEANceHYe9YALv-Lkm_pd1K4zyhaeV8RlXJ-jfusexf</t>
+        </is>
+      </c>
+      <c r="V214">
+        <v>6297</v>
+      </c>
+      <c r="W214" t="inlineStr">
+        <is>
+          <t>SERVICOS DE CONFECCAO DE PECAS E ACESSORIOS DE ACRILICO EM GERAL.</t>
+        </is>
+      </c>
+      <c r="X214">
+        <v>2321</v>
+      </c>
+      <c r="Y214" t="inlineStr">
+        <is>
+          <t>FUNDACAO CENTRO DE HEMATOLOGIA E HEMOTERAPIA DE MINAS GERAIS</t>
+        </is>
+      </c>
+      <c r="Z214" t="inlineStr">
+        <is>
+          <t>SERVICOS DE CONFECCAO DE ARTEFATOS DE ACRILICO</t>
+        </is>
+      </c>
+      <c r="AA214" t="inlineStr">
+        <is>
+          <t>MINAS GERAIS</t>
+        </is>
+      </c>
+      <c r="AB214">
+        <v>0</v>
+      </c>
+      <c r="AC214">
+        <v>9972</v>
+      </c>
+      <c r="AD214">
+        <v>8496</v>
+      </c>
+      <c r="AE214">
+        <v>9972</v>
+      </c>
+      <c r="AF214">
+        <v>8496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>